<commit_message>
testing results, SQL stuff
</commit_message>
<xml_diff>
--- a/Testing Results.xlsx
+++ b/Testing Results.xlsx
@@ -1,25 +1,69 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\i-was-abandoned-lol\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BF4ED2-6796-469E-81FD-907BB4C3B9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E15334D4-E9A2-4E96-BCC3-770CFC6854C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Test ID</t>
+  </si>
+  <si>
+    <t>Created By</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>Elliot</t>
+  </si>
+  <si>
+    <t>Tests Link</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -85,7 +129,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -97,7 +141,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -144,6 +188,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -179,6 +240,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -330,13 +408,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE40C47-554B-4126-8700-F46D54D1AEE5}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Literally can't stay awake; good night
</commit_message>
<xml_diff>
--- a/Testing Results.xlsx
+++ b/Testing Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\i-was-abandoned-lol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB98887-8C18-461D-8A01-03C308945627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA2BF41-BDC1-4FA3-8469-BB5775DE6194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1572" yWindow="2916" windowWidth="17280" windowHeight="6948" xr2:uid="{E15334D4-E9A2-4E96-BCC3-770CFC6854C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>Test ID</t>
   </si>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE40C47-554B-4126-8700-F46D54D1AEE5}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,6 +559,9 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -570,6 +573,9 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -581,6 +587,9 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -592,6 +601,9 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -603,6 +615,9 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -614,6 +629,9 @@
       <c r="C9" t="s">
         <v>21</v>
       </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -625,6 +643,9 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -636,6 +657,9 @@
       <c r="C11" t="s">
         <v>25</v>
       </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -647,6 +671,9 @@
       <c r="C12" t="s">
         <v>27</v>
       </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -658,6 +685,9 @@
       <c r="C13" t="s">
         <v>28</v>
       </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -669,6 +699,9 @@
       <c r="C14" t="s">
         <v>30</v>
       </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -680,6 +713,9 @@
       <c r="C15" t="s">
         <v>32</v>
       </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -690,6 +726,9 @@
       </c>
       <c r="C16" t="s">
         <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>